<commit_message>
dopisanie dodatkow do raportu
</commit_message>
<xml_diff>
--- a/App/Raport.xlsx
+++ b/App/Raport.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poreb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm\Desktop\Projekt_DW\DW\App\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Zadania</t>
   </si>
@@ -144,12 +144,15 @@
   </si>
   <si>
     <t>Suma</t>
+  </si>
+  <si>
+    <t>Dodatki do aplikacji + wsp. Elementów</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,12 +162,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -179,11 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -495,20 +505,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:L20"/>
+  <dimension ref="C2:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -531,7 +541,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>3</v>
       </c>
@@ -551,8 +561,8 @@
         <v>28</v>
       </c>
       <c r="I3">
-        <f>9+7.5+3.5+1+3</f>
-        <v>24</v>
+        <f>9+7.5+3.5+1+3+4</f>
+        <v>28</v>
       </c>
       <c r="J3">
         <f>0.5+1.5+1+1+1.5+4+4</f>
@@ -560,13 +570,13 @@
       </c>
       <c r="K3">
         <f>SUM(G3:J3)</f>
-        <v>93.5</v>
+        <v>97.5</v>
       </c>
       <c r="L3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -578,25 +588,25 @@
       </c>
       <c r="G4">
         <f>G3/K3*100</f>
-        <v>29.946524064171122</v>
+        <v>28.717948717948715</v>
       </c>
       <c r="H4">
         <f>H3/K3*100</f>
-        <v>29.946524064171122</v>
+        <v>28.717948717948715</v>
       </c>
       <c r="I4">
         <f>I3/K3*100</f>
-        <v>25.668449197860966</v>
+        <v>28.717948717948715</v>
       </c>
       <c r="J4">
         <f>J3/K3*100</f>
-        <v>14.438502673796791</v>
+        <v>13.846153846153847</v>
       </c>
       <c r="L4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -608,165 +618,177 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>22</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>23</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>